<commit_message>
working script updated, thanks chatGPT
</commit_message>
<xml_diff>
--- a/sprint_tracker.xlsx
+++ b/sprint_tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayode\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayode\staffde-6months-sprint-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807ABF5F-44C3-42D4-B4BC-F2F5EF687293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22271836-C860-4801-BC00-4AEB5CAF8D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="125">
   <si>
     <t>Time</t>
   </si>
@@ -772,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D824062-D0BB-4101-960F-BEFFEEBD67A0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1143,7 +1143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1165,21 +1167,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>45769</v>
-      </c>
-      <c r="B2">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>